<commit_message>
fix bad date MHNA UD
</commit_message>
<xml_diff>
--- a/import_files/output_files/MHNA_ud_processed.xlsx
+++ b/import_files/output_files/MHNA_ud_processed.xlsx
@@ -11237,7 +11237,7 @@
     <t xml:space="preserve">AR-MHNA-EFW01-UD-472</t>
   </si>
   <si>
-    <t xml:space="preserve">1910-1873</t>
+    <t xml:space="preserve">1873-1910</t>
   </si>
   <si>
     <t xml:space="preserve">completo | incompleto</t>
@@ -11351,7 +11351,7 @@
     <t xml:space="preserve">AR-MHNA-EFW01-UD-475</t>
   </si>
   <si>
-    <t xml:space="preserve">1913-1870</t>
+    <t xml:space="preserve">1870-1913</t>
   </si>
   <si>
     <t xml:space="preserve">Si bien los recortes refieren a 1870 (cuando se recibió de Doctor), 1890 (su viaje al exterior), con el tarjetón personal del final se asignó una fecha extrema más amplia. 2023/06/23</t>
@@ -11845,8 +11845,8 @@
   </sheetPr>
   <dimension ref="A1:BI473"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A446" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O476" activeCellId="0" sqref="O476"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A437" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P466" activeCellId="0" sqref="P466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>